<commit_message>
Partially implement Folder migration
Implementation of Processes, Assets and Queues
English version only
</commit_message>
<xml_diff>
--- a/Workbooks/EN/Folders.xlsx
+++ b/Workbooks/EN/Folders.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Workbooks\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F9A2A06-5365-44EE-AA81-23124DBB6A8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{319ECFD1-B2FE-45F3-9D90-871EE0C55745}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Get" sheetId="4" r:id="rId1"/>
     <sheet name="Create" sheetId="1" r:id="rId2"/>
     <sheet name="Delete" sheetId="2" r:id="rId3"/>
+    <sheet name="Migrate Classic to Modern" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>ID</t>
   </si>
@@ -59,6 +60,27 @@
   </si>
   <si>
     <t>Roles Assignment Model</t>
+  </si>
+  <si>
+    <t>Classic Folder Name</t>
+  </si>
+  <si>
+    <t>Modern Folder Name</t>
+  </si>
+  <si>
+    <t>Environment Migration Policy</t>
+  </si>
+  <si>
+    <t>Queue Migration Policy</t>
+  </si>
+  <si>
+    <t>Asset Migration Policy</t>
+  </si>
+  <si>
+    <t>Robot Migration Policy</t>
+  </si>
+  <si>
+    <t>Process Migration Policy</t>
   </si>
 </sst>
 </file>
@@ -229,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
@@ -274,11 +296,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="26">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -307,52 +330,192 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
-        <patternFill patternType="solid">
+        <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor theme="2"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
+          <color theme="5"/>
         </left>
-        <right style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </right>
+        <right/>
         <top style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
+          <color theme="5"/>
         </top>
         <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
+          <color theme="5"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
-        <patternFill patternType="solid">
+        <patternFill patternType="none">
           <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="5"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="5"/>
+        </top>
+        <bottom style="thin">
+          <color theme="5"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="5"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="5"/>
+        </top>
+        <bottom style="thin">
+          <color theme="5"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="5"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="5"/>
+        </top>
+        <bottom style="thin">
+          <color theme="5"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="5"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="5"/>
+        </top>
+        <bottom style="thin">
+          <color theme="5"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="5"/>
+        </left>
+        <right style="thin">
+          <color theme="5"/>
+        </right>
+        <top style="thin">
+          <color theme="5"/>
+        </top>
+        <bottom style="thin">
+          <color theme="5"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="5"/>
+        </left>
+        <right style="thin">
+          <color theme="5"/>
+        </right>
+        <top style="thin">
+          <color theme="5"/>
+        </top>
+        <bottom style="thin">
+          <color theme="5"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="5"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="5"/>
+        </horizontal>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </bottom>
-      </border>
-      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -432,6 +595,31 @@
         <horizontal style="thin">
           <color theme="5"/>
         </horizontal>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
       </border>
       <protection locked="1" hidden="0"/>
     </dxf>
@@ -552,6 +740,31 @@
           <bgColor theme="2"/>
         </patternFill>
       </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -630,6 +843,31 @@
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -687,15 +925,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:F201" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:F201" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="A1:F201" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Folder ID" totalsRowLabel="Total" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Folder Name" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{09C93F80-4709-492E-B123-1FD1377F6101}" name="Type" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{8B6D5F42-D711-499A-B47F-11E353F96F8A}" name="Roles Assignment Model" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{13860EF0-E108-453A-B4F0-BF4407F583EB}" name="Parent Folder ID" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{75FE23B7-3A10-47F6-A482-B742DB549888}" name="Parent Folder Name" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Folder ID" totalsRowLabel="Total" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Folder Name" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{09C93F80-4709-492E-B123-1FD1377F6101}" name="Type" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{8B6D5F42-D711-499A-B47F-11E353F96F8A}" name="Roles Assignment Model" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{13860EF0-E108-453A-B4F0-BF4407F583EB}" name="Parent Folder ID" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{75FE23B7-3A10-47F6-A482-B742DB549888}" name="Parent Folder Name" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -705,12 +943,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F201" totalsRowShown="0">
   <autoFilter ref="A1:F201" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="6" xr3:uid="{1629EEA8-0A04-47B6-959A-94707301E32E}" name="Type" dataDxfId="10"/>
-    <tableColumn id="1" xr3:uid="{554ACE0F-14A0-4C52-B426-ABC478833011}" name="Folder Name" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{6D933BDD-AD4A-46BD-8368-548E99B8F945}" name="Roles Assignment Model" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Parent Folder Name" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="ID" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{D1E6EAA2-70C4-4033-9FEE-92C367F3E3E4}" name="Result" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{1629EEA8-0A04-47B6-959A-94707301E32E}" name="Type" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{554ACE0F-14A0-4C52-B426-ABC478833011}" name="Folder Name" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{6D933BDD-AD4A-46BD-8368-548E99B8F945}" name="Roles Assignment Model" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Parent Folder Name" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="ID" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{D1E6EAA2-70C4-4033-9FEE-92C367F3E3E4}" name="Result" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -720,9 +958,26 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:C201" totalsRowShown="0">
   <autoFilter ref="A1:C201" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Folder ID" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{77482336-B9C3-42EA-B117-2D0B1D764C3A}" name="Folder Name" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{9F11D09F-EBB8-481F-9883-602BE1C1BEC7}" name="Result" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Folder ID" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{77482336-B9C3-42EA-B117-2D0B1D764C3A}" name="Folder Name" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{9F11D09F-EBB8-481F-9883-602BE1C1BEC7}" name="Result" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C741A763-C973-4E3D-9667-E279531D029B}" name="Table135" displayName="Table135" ref="A1:H201" totalsRowShown="0">
+  <autoFilter ref="A1:H201" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{06DA14B0-5E22-4EEF-A18B-A35402B004D6}" name="Classic Folder Name" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{26AAE292-FD7A-4736-9665-4C3F4F2E4691}" name="Environment Migration Policy" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{8B67F779-E5D4-454F-B1AE-BDF759F343F5}" name="Modern Folder Name" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{544CD008-7B91-4BD3-92D4-DA1FBA78F88E}" name="Process Migration Policy" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{03D952F5-9916-4976-9092-1E205FF9B082}" name="Asset Migration Policy" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{408FB860-E517-4375-BDC7-0BE41F885425}" name="Queue Migration Policy" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{2B291FE3-6124-4687-97DD-58D1D1D26077}" name="Robot Migration Policy" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{38CA2D2B-A2DD-4A97-B630-520A89F12C7B}" name="Result" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -993,7 +1248,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2B90804-4CC2-4F3A-A5A0-B313E9BACDDF}">
   <dimension ref="A1:F201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -5348,4 +5603,2090 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8DD3B9-D83D-408E-AEF0-E69491DEC7A2}">
+  <dimension ref="A1:H201"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.81640625" customWidth="1"/>
+    <col min="3" max="3" width="22.7265625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="23.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.08984375" customWidth="1"/>
+    <col min="9" max="9" width="8.36328125" customWidth="1"/>
+    <col min="10" max="10" width="8.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="7"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="7"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="7"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="7"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="7"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="7"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="7"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="7"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="7"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="6"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="6"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="6"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="6"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="6"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="6"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="6"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="6"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="6"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="6"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="6"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="6"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="6"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="6"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="6"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="6"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="6"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="6"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="6"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="6"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" s="6"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" s="6"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" s="6"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="4"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" s="6"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="4"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="6"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="4"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" s="6"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" s="6"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" s="6"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A39" s="6"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A40" s="6"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41" s="6"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A42" s="6"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A43" s="6"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44" s="6"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45" s="6"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A46" s="6"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="4"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A47" s="6"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="19"/>
+      <c r="H47" s="4"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A48" s="6"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="4"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A49" s="6"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="19"/>
+      <c r="H49" s="4"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A50" s="6"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="4"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A51" s="6"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="19"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="4"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A52" s="6"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="19"/>
+      <c r="G52" s="19"/>
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A53" s="6"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="19"/>
+      <c r="G53" s="19"/>
+      <c r="H53" s="4"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A54" s="6"/>
+      <c r="B54" s="8"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="19"/>
+      <c r="F54" s="19"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="4"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A55" s="6"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="19"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="19"/>
+      <c r="G55" s="19"/>
+      <c r="H55" s="4"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A56" s="6"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="19"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="19"/>
+      <c r="G56" s="19"/>
+      <c r="H56" s="4"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A57" s="6"/>
+      <c r="B57" s="8"/>
+      <c r="C57" s="19"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="19"/>
+      <c r="G57" s="19"/>
+      <c r="H57" s="4"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A58" s="6"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="19"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="19"/>
+      <c r="F58" s="19"/>
+      <c r="G58" s="19"/>
+      <c r="H58" s="4"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A59" s="6"/>
+      <c r="B59" s="8"/>
+      <c r="C59" s="19"/>
+      <c r="D59" s="19"/>
+      <c r="E59" s="19"/>
+      <c r="F59" s="19"/>
+      <c r="G59" s="19"/>
+      <c r="H59" s="4"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A60" s="6"/>
+      <c r="B60" s="8"/>
+      <c r="C60" s="19"/>
+      <c r="D60" s="19"/>
+      <c r="E60" s="19"/>
+      <c r="F60" s="19"/>
+      <c r="G60" s="19"/>
+      <c r="H60" s="4"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A61" s="6"/>
+      <c r="B61" s="8"/>
+      <c r="C61" s="19"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="19"/>
+      <c r="F61" s="19"/>
+      <c r="G61" s="19"/>
+      <c r="H61" s="4"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A62" s="6"/>
+      <c r="B62" s="8"/>
+      <c r="C62" s="19"/>
+      <c r="D62" s="19"/>
+      <c r="E62" s="19"/>
+      <c r="F62" s="19"/>
+      <c r="G62" s="19"/>
+      <c r="H62" s="4"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A63" s="6"/>
+      <c r="B63" s="8"/>
+      <c r="C63" s="19"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="19"/>
+      <c r="F63" s="19"/>
+      <c r="G63" s="19"/>
+      <c r="H63" s="4"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A64" s="6"/>
+      <c r="B64" s="8"/>
+      <c r="C64" s="19"/>
+      <c r="D64" s="19"/>
+      <c r="E64" s="19"/>
+      <c r="F64" s="19"/>
+      <c r="G64" s="19"/>
+      <c r="H64" s="4"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A65" s="6"/>
+      <c r="B65" s="8"/>
+      <c r="C65" s="19"/>
+      <c r="D65" s="19"/>
+      <c r="E65" s="19"/>
+      <c r="F65" s="19"/>
+      <c r="G65" s="19"/>
+      <c r="H65" s="4"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A66" s="6"/>
+      <c r="B66" s="8"/>
+      <c r="C66" s="19"/>
+      <c r="D66" s="19"/>
+      <c r="E66" s="19"/>
+      <c r="F66" s="19"/>
+      <c r="G66" s="19"/>
+      <c r="H66" s="4"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A67" s="6"/>
+      <c r="B67" s="8"/>
+      <c r="C67" s="19"/>
+      <c r="D67" s="19"/>
+      <c r="E67" s="19"/>
+      <c r="F67" s="19"/>
+      <c r="G67" s="19"/>
+      <c r="H67" s="4"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A68" s="6"/>
+      <c r="B68" s="8"/>
+      <c r="C68" s="19"/>
+      <c r="D68" s="19"/>
+      <c r="E68" s="19"/>
+      <c r="F68" s="19"/>
+      <c r="G68" s="19"/>
+      <c r="H68" s="4"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A69" s="6"/>
+      <c r="B69" s="8"/>
+      <c r="C69" s="19"/>
+      <c r="D69" s="19"/>
+      <c r="E69" s="19"/>
+      <c r="F69" s="19"/>
+      <c r="G69" s="19"/>
+      <c r="H69" s="4"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A70" s="6"/>
+      <c r="B70" s="8"/>
+      <c r="C70" s="19"/>
+      <c r="D70" s="19"/>
+      <c r="E70" s="19"/>
+      <c r="F70" s="19"/>
+      <c r="G70" s="19"/>
+      <c r="H70" s="4"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A71" s="6"/>
+      <c r="B71" s="8"/>
+      <c r="C71" s="19"/>
+      <c r="D71" s="19"/>
+      <c r="E71" s="19"/>
+      <c r="F71" s="19"/>
+      <c r="G71" s="19"/>
+      <c r="H71" s="4"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A72" s="6"/>
+      <c r="B72" s="8"/>
+      <c r="C72" s="19"/>
+      <c r="D72" s="19"/>
+      <c r="E72" s="19"/>
+      <c r="F72" s="19"/>
+      <c r="G72" s="19"/>
+      <c r="H72" s="4"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A73" s="6"/>
+      <c r="B73" s="8"/>
+      <c r="C73" s="19"/>
+      <c r="D73" s="19"/>
+      <c r="E73" s="19"/>
+      <c r="F73" s="19"/>
+      <c r="G73" s="19"/>
+      <c r="H73" s="4"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A74" s="6"/>
+      <c r="B74" s="8"/>
+      <c r="C74" s="19"/>
+      <c r="D74" s="19"/>
+      <c r="E74" s="19"/>
+      <c r="F74" s="19"/>
+      <c r="G74" s="19"/>
+      <c r="H74" s="4"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A75" s="6"/>
+      <c r="B75" s="8"/>
+      <c r="C75" s="19"/>
+      <c r="D75" s="19"/>
+      <c r="E75" s="19"/>
+      <c r="F75" s="19"/>
+      <c r="G75" s="19"/>
+      <c r="H75" s="4"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A76" s="6"/>
+      <c r="B76" s="8"/>
+      <c r="C76" s="19"/>
+      <c r="D76" s="19"/>
+      <c r="E76" s="19"/>
+      <c r="F76" s="19"/>
+      <c r="G76" s="19"/>
+      <c r="H76" s="4"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A77" s="6"/>
+      <c r="B77" s="8"/>
+      <c r="C77" s="19"/>
+      <c r="D77" s="19"/>
+      <c r="E77" s="19"/>
+      <c r="F77" s="19"/>
+      <c r="G77" s="19"/>
+      <c r="H77" s="4"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A78" s="6"/>
+      <c r="B78" s="8"/>
+      <c r="C78" s="19"/>
+      <c r="D78" s="19"/>
+      <c r="E78" s="19"/>
+      <c r="F78" s="19"/>
+      <c r="G78" s="19"/>
+      <c r="H78" s="4"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A79" s="6"/>
+      <c r="B79" s="8"/>
+      <c r="C79" s="19"/>
+      <c r="D79" s="19"/>
+      <c r="E79" s="19"/>
+      <c r="F79" s="19"/>
+      <c r="G79" s="19"/>
+      <c r="H79" s="4"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A80" s="6"/>
+      <c r="B80" s="8"/>
+      <c r="C80" s="19"/>
+      <c r="D80" s="19"/>
+      <c r="E80" s="19"/>
+      <c r="F80" s="19"/>
+      <c r="G80" s="19"/>
+      <c r="H80" s="4"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A81" s="6"/>
+      <c r="B81" s="6"/>
+      <c r="C81" s="19"/>
+      <c r="D81" s="19"/>
+      <c r="E81" s="19"/>
+      <c r="F81" s="19"/>
+      <c r="G81" s="19"/>
+      <c r="H81" s="4"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A82" s="6"/>
+      <c r="B82" s="6"/>
+      <c r="C82" s="19"/>
+      <c r="D82" s="19"/>
+      <c r="E82" s="19"/>
+      <c r="F82" s="19"/>
+      <c r="G82" s="19"/>
+      <c r="H82" s="4"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A83" s="6"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="19"/>
+      <c r="D83" s="19"/>
+      <c r="E83" s="19"/>
+      <c r="F83" s="19"/>
+      <c r="G83" s="19"/>
+      <c r="H83" s="4"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A84" s="6"/>
+      <c r="B84" s="6"/>
+      <c r="C84" s="19"/>
+      <c r="D84" s="19"/>
+      <c r="E84" s="19"/>
+      <c r="F84" s="19"/>
+      <c r="G84" s="19"/>
+      <c r="H84" s="4"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A85" s="6"/>
+      <c r="B85" s="6"/>
+      <c r="C85" s="19"/>
+      <c r="D85" s="19"/>
+      <c r="E85" s="19"/>
+      <c r="F85" s="19"/>
+      <c r="G85" s="19"/>
+      <c r="H85" s="4"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A86" s="6"/>
+      <c r="B86" s="6"/>
+      <c r="C86" s="19"/>
+      <c r="D86" s="19"/>
+      <c r="E86" s="19"/>
+      <c r="F86" s="19"/>
+      <c r="G86" s="19"/>
+      <c r="H86" s="4"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A87" s="6"/>
+      <c r="B87" s="6"/>
+      <c r="C87" s="19"/>
+      <c r="D87" s="19"/>
+      <c r="E87" s="19"/>
+      <c r="F87" s="19"/>
+      <c r="G87" s="19"/>
+      <c r="H87" s="4"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A88" s="6"/>
+      <c r="B88" s="6"/>
+      <c r="C88" s="19"/>
+      <c r="D88" s="19"/>
+      <c r="E88" s="19"/>
+      <c r="F88" s="19"/>
+      <c r="G88" s="19"/>
+      <c r="H88" s="4"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A89" s="6"/>
+      <c r="B89" s="6"/>
+      <c r="C89" s="19"/>
+      <c r="D89" s="19"/>
+      <c r="E89" s="19"/>
+      <c r="F89" s="19"/>
+      <c r="G89" s="19"/>
+      <c r="H89" s="4"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A90" s="6"/>
+      <c r="B90" s="6"/>
+      <c r="C90" s="19"/>
+      <c r="D90" s="19"/>
+      <c r="E90" s="19"/>
+      <c r="F90" s="19"/>
+      <c r="G90" s="19"/>
+      <c r="H90" s="4"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A91" s="6"/>
+      <c r="B91" s="6"/>
+      <c r="C91" s="19"/>
+      <c r="D91" s="19"/>
+      <c r="E91" s="19"/>
+      <c r="F91" s="19"/>
+      <c r="G91" s="19"/>
+      <c r="H91" s="4"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A92" s="6"/>
+      <c r="B92" s="6"/>
+      <c r="C92" s="19"/>
+      <c r="D92" s="19"/>
+      <c r="E92" s="19"/>
+      <c r="F92" s="19"/>
+      <c r="G92" s="19"/>
+      <c r="H92" s="4"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A93" s="6"/>
+      <c r="B93" s="6"/>
+      <c r="C93" s="19"/>
+      <c r="D93" s="19"/>
+      <c r="E93" s="19"/>
+      <c r="F93" s="19"/>
+      <c r="G93" s="19"/>
+      <c r="H93" s="4"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A94" s="6"/>
+      <c r="B94" s="6"/>
+      <c r="C94" s="19"/>
+      <c r="D94" s="19"/>
+      <c r="E94" s="19"/>
+      <c r="F94" s="19"/>
+      <c r="G94" s="19"/>
+      <c r="H94" s="4"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A95" s="6"/>
+      <c r="B95" s="6"/>
+      <c r="C95" s="19"/>
+      <c r="D95" s="19"/>
+      <c r="E95" s="19"/>
+      <c r="F95" s="19"/>
+      <c r="G95" s="19"/>
+      <c r="H95" s="4"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A96" s="6"/>
+      <c r="B96" s="6"/>
+      <c r="C96" s="19"/>
+      <c r="D96" s="19"/>
+      <c r="E96" s="19"/>
+      <c r="F96" s="19"/>
+      <c r="G96" s="19"/>
+      <c r="H96" s="4"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A97" s="6"/>
+      <c r="B97" s="6"/>
+      <c r="C97" s="19"/>
+      <c r="D97" s="19"/>
+      <c r="E97" s="19"/>
+      <c r="F97" s="19"/>
+      <c r="G97" s="19"/>
+      <c r="H97" s="4"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A98" s="6"/>
+      <c r="B98" s="6"/>
+      <c r="C98" s="19"/>
+      <c r="D98" s="19"/>
+      <c r="E98" s="19"/>
+      <c r="F98" s="19"/>
+      <c r="G98" s="19"/>
+      <c r="H98" s="4"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A99" s="6"/>
+      <c r="B99" s="6"/>
+      <c r="C99" s="19"/>
+      <c r="D99" s="19"/>
+      <c r="E99" s="19"/>
+      <c r="F99" s="19"/>
+      <c r="G99" s="19"/>
+      <c r="H99" s="4"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A100" s="6"/>
+      <c r="B100" s="6"/>
+      <c r="C100" s="19"/>
+      <c r="D100" s="19"/>
+      <c r="E100" s="19"/>
+      <c r="F100" s="19"/>
+      <c r="G100" s="19"/>
+      <c r="H100" s="4"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A101" s="6"/>
+      <c r="B101" s="6"/>
+      <c r="C101" s="19"/>
+      <c r="D101" s="19"/>
+      <c r="E101" s="19"/>
+      <c r="F101" s="19"/>
+      <c r="G101" s="19"/>
+      <c r="H101" s="4"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A102" s="6"/>
+      <c r="B102" s="6"/>
+      <c r="C102" s="19"/>
+      <c r="D102" s="19"/>
+      <c r="E102" s="19"/>
+      <c r="F102" s="19"/>
+      <c r="G102" s="19"/>
+      <c r="H102" s="4"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A103" s="6"/>
+      <c r="B103" s="6"/>
+      <c r="C103" s="19"/>
+      <c r="D103" s="19"/>
+      <c r="E103" s="19"/>
+      <c r="F103" s="19"/>
+      <c r="G103" s="19"/>
+      <c r="H103" s="4"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A104" s="6"/>
+      <c r="B104" s="6"/>
+      <c r="C104" s="19"/>
+      <c r="D104" s="19"/>
+      <c r="E104" s="19"/>
+      <c r="F104" s="19"/>
+      <c r="G104" s="19"/>
+      <c r="H104" s="4"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A105" s="6"/>
+      <c r="B105" s="6"/>
+      <c r="C105" s="19"/>
+      <c r="D105" s="19"/>
+      <c r="E105" s="19"/>
+      <c r="F105" s="19"/>
+      <c r="G105" s="19"/>
+      <c r="H105" s="4"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A106" s="6"/>
+      <c r="B106" s="6"/>
+      <c r="C106" s="19"/>
+      <c r="D106" s="19"/>
+      <c r="E106" s="19"/>
+      <c r="F106" s="19"/>
+      <c r="G106" s="19"/>
+      <c r="H106" s="4"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A107" s="6"/>
+      <c r="B107" s="6"/>
+      <c r="C107" s="19"/>
+      <c r="D107" s="19"/>
+      <c r="E107" s="19"/>
+      <c r="F107" s="19"/>
+      <c r="G107" s="19"/>
+      <c r="H107" s="4"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A108" s="6"/>
+      <c r="B108" s="6"/>
+      <c r="C108" s="19"/>
+      <c r="D108" s="19"/>
+      <c r="E108" s="19"/>
+      <c r="F108" s="19"/>
+      <c r="G108" s="19"/>
+      <c r="H108" s="4"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A109" s="6"/>
+      <c r="B109" s="6"/>
+      <c r="C109" s="19"/>
+      <c r="D109" s="19"/>
+      <c r="E109" s="19"/>
+      <c r="F109" s="19"/>
+      <c r="G109" s="19"/>
+      <c r="H109" s="4"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A110" s="6"/>
+      <c r="B110" s="6"/>
+      <c r="C110" s="19"/>
+      <c r="D110" s="19"/>
+      <c r="E110" s="19"/>
+      <c r="F110" s="19"/>
+      <c r="G110" s="19"/>
+      <c r="H110" s="4"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A111" s="6"/>
+      <c r="B111" s="6"/>
+      <c r="C111" s="19"/>
+      <c r="D111" s="19"/>
+      <c r="E111" s="19"/>
+      <c r="F111" s="19"/>
+      <c r="G111" s="19"/>
+      <c r="H111" s="4"/>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A112" s="6"/>
+      <c r="B112" s="6"/>
+      <c r="C112" s="19"/>
+      <c r="D112" s="19"/>
+      <c r="E112" s="19"/>
+      <c r="F112" s="19"/>
+      <c r="G112" s="19"/>
+      <c r="H112" s="4"/>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A113" s="6"/>
+      <c r="B113" s="6"/>
+      <c r="C113" s="19"/>
+      <c r="D113" s="19"/>
+      <c r="E113" s="19"/>
+      <c r="F113" s="19"/>
+      <c r="G113" s="19"/>
+      <c r="H113" s="4"/>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A114" s="6"/>
+      <c r="B114" s="6"/>
+      <c r="C114" s="19"/>
+      <c r="D114" s="19"/>
+      <c r="E114" s="19"/>
+      <c r="F114" s="19"/>
+      <c r="G114" s="19"/>
+      <c r="H114" s="4"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A115" s="6"/>
+      <c r="B115" s="6"/>
+      <c r="C115" s="19"/>
+      <c r="D115" s="19"/>
+      <c r="E115" s="19"/>
+      <c r="F115" s="19"/>
+      <c r="G115" s="19"/>
+      <c r="H115" s="4"/>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A116" s="6"/>
+      <c r="B116" s="6"/>
+      <c r="C116" s="19"/>
+      <c r="D116" s="19"/>
+      <c r="E116" s="19"/>
+      <c r="F116" s="19"/>
+      <c r="G116" s="19"/>
+      <c r="H116" s="4"/>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A117" s="6"/>
+      <c r="B117" s="6"/>
+      <c r="C117" s="19"/>
+      <c r="D117" s="19"/>
+      <c r="E117" s="19"/>
+      <c r="F117" s="19"/>
+      <c r="G117" s="19"/>
+      <c r="H117" s="4"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A118" s="6"/>
+      <c r="B118" s="6"/>
+      <c r="C118" s="19"/>
+      <c r="D118" s="19"/>
+      <c r="E118" s="19"/>
+      <c r="F118" s="19"/>
+      <c r="G118" s="19"/>
+      <c r="H118" s="4"/>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A119" s="6"/>
+      <c r="B119" s="6"/>
+      <c r="C119" s="19"/>
+      <c r="D119" s="19"/>
+      <c r="E119" s="19"/>
+      <c r="F119" s="19"/>
+      <c r="G119" s="19"/>
+      <c r="H119" s="4"/>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A120" s="6"/>
+      <c r="B120" s="6"/>
+      <c r="C120" s="19"/>
+      <c r="D120" s="19"/>
+      <c r="E120" s="19"/>
+      <c r="F120" s="19"/>
+      <c r="G120" s="19"/>
+      <c r="H120" s="4"/>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A121" s="6"/>
+      <c r="B121" s="6"/>
+      <c r="C121" s="19"/>
+      <c r="D121" s="19"/>
+      <c r="E121" s="19"/>
+      <c r="F121" s="19"/>
+      <c r="G121" s="19"/>
+      <c r="H121" s="4"/>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A122" s="6"/>
+      <c r="B122" s="6"/>
+      <c r="C122" s="19"/>
+      <c r="D122" s="19"/>
+      <c r="E122" s="19"/>
+      <c r="F122" s="19"/>
+      <c r="G122" s="19"/>
+      <c r="H122" s="4"/>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A123" s="6"/>
+      <c r="B123" s="6"/>
+      <c r="C123" s="19"/>
+      <c r="D123" s="19"/>
+      <c r="E123" s="19"/>
+      <c r="F123" s="19"/>
+      <c r="G123" s="19"/>
+      <c r="H123" s="4"/>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A124" s="6"/>
+      <c r="B124" s="6"/>
+      <c r="C124" s="19"/>
+      <c r="D124" s="19"/>
+      <c r="E124" s="19"/>
+      <c r="F124" s="19"/>
+      <c r="G124" s="19"/>
+      <c r="H124" s="4"/>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A125" s="6"/>
+      <c r="B125" s="6"/>
+      <c r="C125" s="19"/>
+      <c r="D125" s="19"/>
+      <c r="E125" s="19"/>
+      <c r="F125" s="19"/>
+      <c r="G125" s="19"/>
+      <c r="H125" s="4"/>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A126" s="6"/>
+      <c r="B126" s="6"/>
+      <c r="C126" s="19"/>
+      <c r="D126" s="19"/>
+      <c r="E126" s="19"/>
+      <c r="F126" s="19"/>
+      <c r="G126" s="19"/>
+      <c r="H126" s="4"/>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A127" s="6"/>
+      <c r="B127" s="6"/>
+      <c r="C127" s="19"/>
+      <c r="D127" s="19"/>
+      <c r="E127" s="19"/>
+      <c r="F127" s="19"/>
+      <c r="G127" s="19"/>
+      <c r="H127" s="4"/>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A128" s="6"/>
+      <c r="B128" s="6"/>
+      <c r="C128" s="19"/>
+      <c r="D128" s="19"/>
+      <c r="E128" s="19"/>
+      <c r="F128" s="19"/>
+      <c r="G128" s="19"/>
+      <c r="H128" s="4"/>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A129" s="6"/>
+      <c r="B129" s="6"/>
+      <c r="C129" s="19"/>
+      <c r="D129" s="19"/>
+      <c r="E129" s="19"/>
+      <c r="F129" s="19"/>
+      <c r="G129" s="19"/>
+      <c r="H129" s="4"/>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A130" s="6"/>
+      <c r="B130" s="6"/>
+      <c r="C130" s="19"/>
+      <c r="D130" s="19"/>
+      <c r="E130" s="19"/>
+      <c r="F130" s="19"/>
+      <c r="G130" s="19"/>
+      <c r="H130" s="4"/>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A131" s="6"/>
+      <c r="B131" s="6"/>
+      <c r="C131" s="19"/>
+      <c r="D131" s="19"/>
+      <c r="E131" s="19"/>
+      <c r="F131" s="19"/>
+      <c r="G131" s="19"/>
+      <c r="H131" s="4"/>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A132" s="6"/>
+      <c r="B132" s="6"/>
+      <c r="C132" s="19"/>
+      <c r="D132" s="19"/>
+      <c r="E132" s="19"/>
+      <c r="F132" s="19"/>
+      <c r="G132" s="19"/>
+      <c r="H132" s="4"/>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A133" s="6"/>
+      <c r="B133" s="6"/>
+      <c r="C133" s="19"/>
+      <c r="D133" s="19"/>
+      <c r="E133" s="19"/>
+      <c r="F133" s="19"/>
+      <c r="G133" s="19"/>
+      <c r="H133" s="4"/>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A134" s="6"/>
+      <c r="B134" s="6"/>
+      <c r="C134" s="19"/>
+      <c r="D134" s="19"/>
+      <c r="E134" s="19"/>
+      <c r="F134" s="19"/>
+      <c r="G134" s="19"/>
+      <c r="H134" s="4"/>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A135" s="6"/>
+      <c r="B135" s="6"/>
+      <c r="C135" s="19"/>
+      <c r="D135" s="19"/>
+      <c r="E135" s="19"/>
+      <c r="F135" s="19"/>
+      <c r="G135" s="19"/>
+      <c r="H135" s="4"/>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A136" s="6"/>
+      <c r="B136" s="6"/>
+      <c r="C136" s="19"/>
+      <c r="D136" s="19"/>
+      <c r="E136" s="19"/>
+      <c r="F136" s="19"/>
+      <c r="G136" s="19"/>
+      <c r="H136" s="4"/>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A137" s="6"/>
+      <c r="B137" s="6"/>
+      <c r="C137" s="19"/>
+      <c r="D137" s="19"/>
+      <c r="E137" s="19"/>
+      <c r="F137" s="19"/>
+      <c r="G137" s="19"/>
+      <c r="H137" s="4"/>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A138" s="6"/>
+      <c r="B138" s="6"/>
+      <c r="C138" s="19"/>
+      <c r="D138" s="19"/>
+      <c r="E138" s="19"/>
+      <c r="F138" s="19"/>
+      <c r="G138" s="19"/>
+      <c r="H138" s="4"/>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A139" s="6"/>
+      <c r="B139" s="6"/>
+      <c r="C139" s="19"/>
+      <c r="D139" s="19"/>
+      <c r="E139" s="19"/>
+      <c r="F139" s="19"/>
+      <c r="G139" s="19"/>
+      <c r="H139" s="4"/>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A140" s="6"/>
+      <c r="B140" s="6"/>
+      <c r="C140" s="19"/>
+      <c r="D140" s="19"/>
+      <c r="E140" s="19"/>
+      <c r="F140" s="19"/>
+      <c r="G140" s="19"/>
+      <c r="H140" s="4"/>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A141" s="6"/>
+      <c r="B141" s="6"/>
+      <c r="C141" s="19"/>
+      <c r="D141" s="19"/>
+      <c r="E141" s="19"/>
+      <c r="F141" s="19"/>
+      <c r="G141" s="19"/>
+      <c r="H141" s="4"/>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A142" s="6"/>
+      <c r="B142" s="6"/>
+      <c r="C142" s="19"/>
+      <c r="D142" s="19"/>
+      <c r="E142" s="19"/>
+      <c r="F142" s="19"/>
+      <c r="G142" s="19"/>
+      <c r="H142" s="4"/>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A143" s="6"/>
+      <c r="B143" s="6"/>
+      <c r="C143" s="19"/>
+      <c r="D143" s="19"/>
+      <c r="E143" s="19"/>
+      <c r="F143" s="19"/>
+      <c r="G143" s="19"/>
+      <c r="H143" s="4"/>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A144" s="6"/>
+      <c r="B144" s="6"/>
+      <c r="C144" s="19"/>
+      <c r="D144" s="19"/>
+      <c r="E144" s="19"/>
+      <c r="F144" s="19"/>
+      <c r="G144" s="19"/>
+      <c r="H144" s="4"/>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A145" s="6"/>
+      <c r="B145" s="6"/>
+      <c r="C145" s="19"/>
+      <c r="D145" s="19"/>
+      <c r="E145" s="19"/>
+      <c r="F145" s="19"/>
+      <c r="G145" s="19"/>
+      <c r="H145" s="4"/>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A146" s="6"/>
+      <c r="B146" s="6"/>
+      <c r="C146" s="19"/>
+      <c r="D146" s="19"/>
+      <c r="E146" s="19"/>
+      <c r="F146" s="19"/>
+      <c r="G146" s="19"/>
+      <c r="H146" s="4"/>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A147" s="6"/>
+      <c r="B147" s="6"/>
+      <c r="C147" s="19"/>
+      <c r="D147" s="19"/>
+      <c r="E147" s="19"/>
+      <c r="F147" s="19"/>
+      <c r="G147" s="19"/>
+      <c r="H147" s="4"/>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A148" s="6"/>
+      <c r="B148" s="6"/>
+      <c r="C148" s="19"/>
+      <c r="D148" s="19"/>
+      <c r="E148" s="19"/>
+      <c r="F148" s="19"/>
+      <c r="G148" s="19"/>
+      <c r="H148" s="4"/>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A149" s="6"/>
+      <c r="B149" s="6"/>
+      <c r="C149" s="19"/>
+      <c r="D149" s="19"/>
+      <c r="E149" s="19"/>
+      <c r="F149" s="19"/>
+      <c r="G149" s="19"/>
+      <c r="H149" s="4"/>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A150" s="6"/>
+      <c r="B150" s="6"/>
+      <c r="C150" s="19"/>
+      <c r="D150" s="19"/>
+      <c r="E150" s="19"/>
+      <c r="F150" s="19"/>
+      <c r="G150" s="19"/>
+      <c r="H150" s="4"/>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A151" s="6"/>
+      <c r="B151" s="6"/>
+      <c r="C151" s="19"/>
+      <c r="D151" s="19"/>
+      <c r="E151" s="19"/>
+      <c r="F151" s="19"/>
+      <c r="G151" s="19"/>
+      <c r="H151" s="4"/>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A152" s="6"/>
+      <c r="B152" s="6"/>
+      <c r="C152" s="19"/>
+      <c r="D152" s="19"/>
+      <c r="E152" s="19"/>
+      <c r="F152" s="19"/>
+      <c r="G152" s="19"/>
+      <c r="H152" s="4"/>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A153" s="6"/>
+      <c r="B153" s="6"/>
+      <c r="C153" s="19"/>
+      <c r="D153" s="19"/>
+      <c r="E153" s="19"/>
+      <c r="F153" s="19"/>
+      <c r="G153" s="19"/>
+      <c r="H153" s="4"/>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A154" s="6"/>
+      <c r="B154" s="6"/>
+      <c r="C154" s="19"/>
+      <c r="D154" s="19"/>
+      <c r="E154" s="19"/>
+      <c r="F154" s="19"/>
+      <c r="G154" s="19"/>
+      <c r="H154" s="4"/>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A155" s="6"/>
+      <c r="B155" s="6"/>
+      <c r="C155" s="19"/>
+      <c r="D155" s="19"/>
+      <c r="E155" s="19"/>
+      <c r="F155" s="19"/>
+      <c r="G155" s="19"/>
+      <c r="H155" s="4"/>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A156" s="6"/>
+      <c r="B156" s="6"/>
+      <c r="C156" s="19"/>
+      <c r="D156" s="19"/>
+      <c r="E156" s="19"/>
+      <c r="F156" s="19"/>
+      <c r="G156" s="19"/>
+      <c r="H156" s="4"/>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A157" s="6"/>
+      <c r="B157" s="6"/>
+      <c r="C157" s="19"/>
+      <c r="D157" s="19"/>
+      <c r="E157" s="19"/>
+      <c r="F157" s="19"/>
+      <c r="G157" s="19"/>
+      <c r="H157" s="4"/>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A158" s="6"/>
+      <c r="B158" s="6"/>
+      <c r="C158" s="19"/>
+      <c r="D158" s="19"/>
+      <c r="E158" s="19"/>
+      <c r="F158" s="19"/>
+      <c r="G158" s="19"/>
+      <c r="H158" s="4"/>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A159" s="6"/>
+      <c r="B159" s="6"/>
+      <c r="C159" s="19"/>
+      <c r="D159" s="19"/>
+      <c r="E159" s="19"/>
+      <c r="F159" s="19"/>
+      <c r="G159" s="19"/>
+      <c r="H159" s="4"/>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A160" s="6"/>
+      <c r="B160" s="6"/>
+      <c r="C160" s="19"/>
+      <c r="D160" s="19"/>
+      <c r="E160" s="19"/>
+      <c r="F160" s="19"/>
+      <c r="G160" s="19"/>
+      <c r="H160" s="4"/>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A161" s="6"/>
+      <c r="B161" s="6"/>
+      <c r="C161" s="19"/>
+      <c r="D161" s="19"/>
+      <c r="E161" s="19"/>
+      <c r="F161" s="19"/>
+      <c r="G161" s="19"/>
+      <c r="H161" s="4"/>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A162" s="6"/>
+      <c r="B162" s="6"/>
+      <c r="C162" s="19"/>
+      <c r="D162" s="19"/>
+      <c r="E162" s="19"/>
+      <c r="F162" s="19"/>
+      <c r="G162" s="19"/>
+      <c r="H162" s="4"/>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A163" s="6"/>
+      <c r="B163" s="6"/>
+      <c r="C163" s="19"/>
+      <c r="D163" s="19"/>
+      <c r="E163" s="19"/>
+      <c r="F163" s="19"/>
+      <c r="G163" s="19"/>
+      <c r="H163" s="4"/>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A164" s="6"/>
+      <c r="B164" s="6"/>
+      <c r="C164" s="19"/>
+      <c r="D164" s="19"/>
+      <c r="E164" s="19"/>
+      <c r="F164" s="19"/>
+      <c r="G164" s="19"/>
+      <c r="H164" s="4"/>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A165" s="6"/>
+      <c r="B165" s="6"/>
+      <c r="C165" s="19"/>
+      <c r="D165" s="19"/>
+      <c r="E165" s="19"/>
+      <c r="F165" s="19"/>
+      <c r="G165" s="19"/>
+      <c r="H165" s="4"/>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A166" s="6"/>
+      <c r="B166" s="6"/>
+      <c r="C166" s="19"/>
+      <c r="D166" s="19"/>
+      <c r="E166" s="19"/>
+      <c r="F166" s="19"/>
+      <c r="G166" s="19"/>
+      <c r="H166" s="4"/>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A167" s="6"/>
+      <c r="B167" s="6"/>
+      <c r="C167" s="19"/>
+      <c r="D167" s="19"/>
+      <c r="E167" s="19"/>
+      <c r="F167" s="19"/>
+      <c r="G167" s="19"/>
+      <c r="H167" s="4"/>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A168" s="6"/>
+      <c r="B168" s="6"/>
+      <c r="C168" s="19"/>
+      <c r="D168" s="19"/>
+      <c r="E168" s="19"/>
+      <c r="F168" s="19"/>
+      <c r="G168" s="19"/>
+      <c r="H168" s="4"/>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A169" s="6"/>
+      <c r="B169" s="6"/>
+      <c r="C169" s="19"/>
+      <c r="D169" s="19"/>
+      <c r="E169" s="19"/>
+      <c r="F169" s="19"/>
+      <c r="G169" s="19"/>
+      <c r="H169" s="4"/>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A170" s="6"/>
+      <c r="B170" s="6"/>
+      <c r="C170" s="19"/>
+      <c r="D170" s="19"/>
+      <c r="E170" s="19"/>
+      <c r="F170" s="19"/>
+      <c r="G170" s="19"/>
+      <c r="H170" s="4"/>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A171" s="6"/>
+      <c r="B171" s="6"/>
+      <c r="C171" s="19"/>
+      <c r="D171" s="19"/>
+      <c r="E171" s="19"/>
+      <c r="F171" s="19"/>
+      <c r="G171" s="19"/>
+      <c r="H171" s="4"/>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A172" s="6"/>
+      <c r="B172" s="6"/>
+      <c r="C172" s="19"/>
+      <c r="D172" s="19"/>
+      <c r="E172" s="19"/>
+      <c r="F172" s="19"/>
+      <c r="G172" s="19"/>
+      <c r="H172" s="4"/>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A173" s="6"/>
+      <c r="B173" s="6"/>
+      <c r="C173" s="19"/>
+      <c r="D173" s="19"/>
+      <c r="E173" s="19"/>
+      <c r="F173" s="19"/>
+      <c r="G173" s="19"/>
+      <c r="H173" s="4"/>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A174" s="6"/>
+      <c r="B174" s="6"/>
+      <c r="C174" s="19"/>
+      <c r="D174" s="19"/>
+      <c r="E174" s="19"/>
+      <c r="F174" s="19"/>
+      <c r="G174" s="19"/>
+      <c r="H174" s="4"/>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A175" s="6"/>
+      <c r="B175" s="6"/>
+      <c r="C175" s="19"/>
+      <c r="D175" s="19"/>
+      <c r="E175" s="19"/>
+      <c r="F175" s="19"/>
+      <c r="G175" s="19"/>
+      <c r="H175" s="4"/>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A176" s="6"/>
+      <c r="B176" s="6"/>
+      <c r="C176" s="19"/>
+      <c r="D176" s="19"/>
+      <c r="E176" s="19"/>
+      <c r="F176" s="19"/>
+      <c r="G176" s="19"/>
+      <c r="H176" s="4"/>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A177" s="6"/>
+      <c r="B177" s="6"/>
+      <c r="C177" s="19"/>
+      <c r="D177" s="19"/>
+      <c r="E177" s="19"/>
+      <c r="F177" s="19"/>
+      <c r="G177" s="19"/>
+      <c r="H177" s="4"/>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A178" s="6"/>
+      <c r="B178" s="6"/>
+      <c r="C178" s="19"/>
+      <c r="D178" s="19"/>
+      <c r="E178" s="19"/>
+      <c r="F178" s="19"/>
+      <c r="G178" s="19"/>
+      <c r="H178" s="4"/>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A179" s="6"/>
+      <c r="B179" s="6"/>
+      <c r="C179" s="19"/>
+      <c r="D179" s="19"/>
+      <c r="E179" s="19"/>
+      <c r="F179" s="19"/>
+      <c r="G179" s="19"/>
+      <c r="H179" s="4"/>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A180" s="6"/>
+      <c r="B180" s="6"/>
+      <c r="C180" s="19"/>
+      <c r="D180" s="19"/>
+      <c r="E180" s="19"/>
+      <c r="F180" s="19"/>
+      <c r="G180" s="19"/>
+      <c r="H180" s="4"/>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A181" s="6"/>
+      <c r="B181" s="6"/>
+      <c r="C181" s="19"/>
+      <c r="D181" s="19"/>
+      <c r="E181" s="19"/>
+      <c r="F181" s="19"/>
+      <c r="G181" s="19"/>
+      <c r="H181" s="4"/>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A182" s="6"/>
+      <c r="B182" s="6"/>
+      <c r="C182" s="19"/>
+      <c r="D182" s="19"/>
+      <c r="E182" s="19"/>
+      <c r="F182" s="19"/>
+      <c r="G182" s="19"/>
+      <c r="H182" s="4"/>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A183" s="6"/>
+      <c r="B183" s="6"/>
+      <c r="C183" s="19"/>
+      <c r="D183" s="19"/>
+      <c r="E183" s="19"/>
+      <c r="F183" s="19"/>
+      <c r="G183" s="19"/>
+      <c r="H183" s="4"/>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A184" s="6"/>
+      <c r="B184" s="6"/>
+      <c r="C184" s="19"/>
+      <c r="D184" s="19"/>
+      <c r="E184" s="19"/>
+      <c r="F184" s="19"/>
+      <c r="G184" s="19"/>
+      <c r="H184" s="4"/>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A185" s="6"/>
+      <c r="B185" s="6"/>
+      <c r="C185" s="19"/>
+      <c r="D185" s="19"/>
+      <c r="E185" s="19"/>
+      <c r="F185" s="19"/>
+      <c r="G185" s="19"/>
+      <c r="H185" s="4"/>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A186" s="6"/>
+      <c r="B186" s="6"/>
+      <c r="C186" s="19"/>
+      <c r="D186" s="19"/>
+      <c r="E186" s="19"/>
+      <c r="F186" s="19"/>
+      <c r="G186" s="19"/>
+      <c r="H186" s="4"/>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A187" s="6"/>
+      <c r="B187" s="6"/>
+      <c r="C187" s="19"/>
+      <c r="D187" s="19"/>
+      <c r="E187" s="19"/>
+      <c r="F187" s="19"/>
+      <c r="G187" s="19"/>
+      <c r="H187" s="4"/>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A188" s="6"/>
+      <c r="B188" s="6"/>
+      <c r="C188" s="19"/>
+      <c r="D188" s="19"/>
+      <c r="E188" s="19"/>
+      <c r="F188" s="19"/>
+      <c r="G188" s="19"/>
+      <c r="H188" s="4"/>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A189" s="6"/>
+      <c r="B189" s="6"/>
+      <c r="C189" s="19"/>
+      <c r="D189" s="19"/>
+      <c r="E189" s="19"/>
+      <c r="F189" s="19"/>
+      <c r="G189" s="19"/>
+      <c r="H189" s="4"/>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A190" s="6"/>
+      <c r="B190" s="6"/>
+      <c r="C190" s="19"/>
+      <c r="D190" s="19"/>
+      <c r="E190" s="19"/>
+      <c r="F190" s="19"/>
+      <c r="G190" s="19"/>
+      <c r="H190" s="4"/>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A191" s="6"/>
+      <c r="B191" s="6"/>
+      <c r="C191" s="19"/>
+      <c r="D191" s="19"/>
+      <c r="E191" s="19"/>
+      <c r="F191" s="19"/>
+      <c r="G191" s="19"/>
+      <c r="H191" s="4"/>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A192" s="6"/>
+      <c r="B192" s="6"/>
+      <c r="C192" s="19"/>
+      <c r="D192" s="19"/>
+      <c r="E192" s="19"/>
+      <c r="F192" s="19"/>
+      <c r="G192" s="19"/>
+      <c r="H192" s="4"/>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A193" s="6"/>
+      <c r="B193" s="6"/>
+      <c r="C193" s="19"/>
+      <c r="D193" s="19"/>
+      <c r="E193" s="19"/>
+      <c r="F193" s="19"/>
+      <c r="G193" s="19"/>
+      <c r="H193" s="4"/>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A194" s="6"/>
+      <c r="B194" s="6"/>
+      <c r="C194" s="19"/>
+      <c r="D194" s="19"/>
+      <c r="E194" s="19"/>
+      <c r="F194" s="19"/>
+      <c r="G194" s="19"/>
+      <c r="H194" s="4"/>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A195" s="6"/>
+      <c r="B195" s="6"/>
+      <c r="C195" s="19"/>
+      <c r="D195" s="19"/>
+      <c r="E195" s="19"/>
+      <c r="F195" s="19"/>
+      <c r="G195" s="19"/>
+      <c r="H195" s="4"/>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A196" s="6"/>
+      <c r="B196" s="6"/>
+      <c r="C196" s="19"/>
+      <c r="D196" s="19"/>
+      <c r="E196" s="19"/>
+      <c r="F196" s="19"/>
+      <c r="G196" s="19"/>
+      <c r="H196" s="4"/>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A197" s="6"/>
+      <c r="B197" s="6"/>
+      <c r="C197" s="19"/>
+      <c r="D197" s="19"/>
+      <c r="E197" s="19"/>
+      <c r="F197" s="19"/>
+      <c r="G197" s="19"/>
+      <c r="H197" s="4"/>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A198" s="6"/>
+      <c r="B198" s="6"/>
+      <c r="C198" s="19"/>
+      <c r="D198" s="19"/>
+      <c r="E198" s="19"/>
+      <c r="F198" s="19"/>
+      <c r="G198" s="19"/>
+      <c r="H198" s="4"/>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A199" s="6"/>
+      <c r="B199" s="6"/>
+      <c r="C199" s="19"/>
+      <c r="D199" s="19"/>
+      <c r="E199" s="19"/>
+      <c r="F199" s="19"/>
+      <c r="G199" s="19"/>
+      <c r="H199" s="4"/>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A200" s="6"/>
+      <c r="B200" s="6"/>
+      <c r="C200" s="19"/>
+      <c r="D200" s="19"/>
+      <c r="E200" s="19"/>
+      <c r="F200" s="19"/>
+      <c r="G200" s="19"/>
+      <c r="H200" s="4"/>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A201" s="10"/>
+      <c r="B201" s="22"/>
+      <c r="C201" s="19"/>
+      <c r="D201" s="19"/>
+      <c r="E201" s="19"/>
+      <c r="F201" s="19"/>
+      <c r="G201" s="19"/>
+      <c r="H201" s="4"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="C2:G201">
+    <cfRule type="expression" dxfId="8" priority="3">
+      <formula>$B2 = "Environments to Different Modern Folders"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E201" xr:uid="{420A1FAB-75A2-4993-B14A-AD369803E7DB}">
+      <formula1>"Migrate Non-Credential Assets,Do Not Migrate Assets"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F201" xr:uid="{1C063541-3E55-41EC-A501-1BF9F4A01EC6}">
+      <formula1>"Migrate All Items,Migrate New Items,Migrate Queue Definitions But Not Queue Items,Do Not Migrate Queues"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E202:E1048576 G2:G201" xr:uid="{8FF33DFF-361F-4A2E-A797-115980BFEA48}">
+      <formula1>"Migrate All Robots,Migrate Only Attended Robots,Migrate Only Unattended Robots,Do Not Migrate Robots"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G202:G1048576" xr:uid="{BA962542-8590-40D3-A410-AD2E2D8342FA}">
+      <formula1>"Migrate All Users,Do Not Migrate Users"</formula1>
+    </dataValidation>
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E201" xr:uid="{63504AD6-A66D-4F41-A4B6-8F8EC15412E5}">
+      <formula1>"Environments to Same Modern Folder,Environments to Different Modern Folders,Do Not Migrate Environments And Processes"</formula1>
+    </dataValidation>
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{761871B1-D5B1-4845-A315-16DA6F2B6705}">
+      <formula1>"Environments to Same Modern Folder,Environments to Different Modern Folders"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{D479BB45-4D1E-431E-809A-21F50FCFBB69}">
+      <formula1>"Migrate All Processes,Do Not Migrate Processes"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implement migration of credential Assets
</commit_message>
<xml_diff>
--- a/Workbooks/EN/Folders.xlsx
+++ b/Workbooks/EN/Folders.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Workbooks\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5D8A97-7765-4990-BEF5-7F991E729795}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9716823-38AF-447E-892F-3B22671C9A20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="799" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14414,7 +14414,7 @@
   </conditionalFormatting>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Migration Policy" error="Please select a supported Asset Migration Policy." sqref="E2:E1048576" xr:uid="{420A1FAB-75A2-4993-B14A-AD369803E7DB}">
-      <formula1>"Migrate Non-Credential Assets,Do Not Migrate Assets"</formula1>
+      <formula1>"Migrate All Assets,Migrate Non-Credential Assets,Do Not Migrate Assets"</formula1>
     </dataValidation>
     <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Migration Policy" error="Please select a supported Environment Migration Policy." sqref="B2:B1048576" xr:uid="{761871B1-D5B1-4845-A315-16DA6F2B6705}">
       <formula1>"Environments to Same Modern Folder,Environments to Different Modern Folders"</formula1>

</xml_diff>